<commit_message>
Add function to join Excel data to feature class
</commit_message>
<xml_diff>
--- a/DesheTools/configuration/classifyTypeCover_Key.xlsx
+++ b/DesheTools/configuration/classifyTypeCover_Key.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tauex-my.sharepoint.com/personal/yoskoyoav_tauex_tau_ac_il/Documents/GIS/PreMapping/OnlineTool/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tauex-my.sharepoint.com/personal/kerenha_tauex_tau_ac_il/Documents/Documents/ArcGIS/Deshe/Deshe/DesheTools/configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1" documentId="8_{D23FDB1F-E947-4AE8-9F3F-3A1A6BF0CD6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55EF0016-9E72-4C43-888B-4AAF1BB2E384}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11235" xr2:uid="{1B3C06EA-3EF4-4486-8996-A04792A06920}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B3C06EA-3EF4-4486-8996-A04792A06920}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -894,21 +894,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC808157-5C55-43DE-9A48-83F916BBB47B}">
   <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -928,7 +928,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>1100</v>
       </c>
@@ -948,7 +948,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>1103</v>
       </c>
@@ -968,7 +968,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>1104</v>
       </c>
@@ -988,7 +988,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>1105</v>
       </c>
@@ -1008,7 +1008,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>1106</v>
       </c>
@@ -1028,7 +1028,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>1191</v>
       </c>
@@ -1046,7 +1046,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="26.5" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>1192</v>
       </c>
@@ -1064,7 +1064,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>1193</v>
       </c>
@@ -1082,7 +1082,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>1200</v>
       </c>
@@ -1102,7 +1102,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>1202</v>
       </c>
@@ -1122,7 +1122,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>1204</v>
       </c>
@@ -1142,7 +1142,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>1310</v>
       </c>
@@ -1162,7 +1162,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>1900</v>
       </c>
@@ -1180,7 +1180,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>1991</v>
       </c>
@@ -1198,7 +1198,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>2000</v>
       </c>
@@ -1216,7 +1216,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>2100</v>
       </c>
@@ -1236,7 +1236,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>2108</v>
       </c>
@@ -1256,7 +1256,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>2113</v>
       </c>
@@ -1276,7 +1276,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>2200</v>
       </c>
@@ -1294,7 +1294,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <v>2211</v>
       </c>
@@ -1314,7 +1314,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>2900</v>
       </c>
@@ -1332,7 +1332,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="3">
         <v>3000</v>
       </c>
@@ -1350,7 +1350,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="3">
         <v>3030</v>
       </c>
@@ -1370,7 +1370,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
         <v>3031</v>
       </c>
@@ -1390,7 +1390,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="3">
         <v>3040</v>
       </c>
@@ -1408,7 +1408,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="3">
         <v>3042</v>
       </c>
@@ -1428,7 +1428,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="3">
         <v>3044</v>
       </c>
@@ -1448,7 +1448,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="3">
         <v>3060</v>
       </c>
@@ -1468,7 +1468,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="3">
         <v>3121</v>
       </c>
@@ -1488,7 +1488,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="3">
         <v>3261</v>
       </c>
@@ -1508,7 +1508,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
         <v>2990</v>
       </c>
@@ -1526,7 +1526,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="3">
         <v>2994</v>
       </c>
@@ -1544,7 +1544,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="3">
         <v>2995</v>
       </c>
@@ -1562,7 +1562,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="3">
         <v>3091</v>
       </c>
@@ -1582,7 +1582,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="3">
         <v>3095</v>
       </c>
@@ -1602,7 +1602,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="3">
         <v>4000</v>
       </c>
@@ -1620,7 +1620,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="3">
         <v>9970</v>
       </c>
@@ -1638,7 +1638,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="26.5" x14ac:dyDescent="0.35">
       <c r="A39" s="3">
         <v>9900</v>
       </c>
@@ -1656,7 +1656,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="3">
         <v>3900</v>
       </c>
@@ -1674,7 +1674,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" s="3">
         <v>3910</v>
       </c>
@@ -1692,7 +1692,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" s="3">
         <v>3920</v>
       </c>
@@ -1710,7 +1710,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" s="3">
         <v>3930</v>
       </c>
@@ -1728,7 +1728,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" s="3">
         <v>3935</v>
       </c>
@@ -1746,7 +1746,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" s="3">
         <v>3940</v>
       </c>
@@ -1764,7 +1764,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" s="3">
         <v>3960</v>
       </c>
@@ -1782,7 +1782,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" s="3">
         <v>3961</v>
       </c>
@@ -1800,7 +1800,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" s="3">
         <v>3962</v>
       </c>
@@ -1818,7 +1818,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" s="3">
         <v>3970</v>
       </c>
@@ -1838,7 +1838,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" s="3">
         <v>3971</v>
       </c>
@@ -1856,7 +1856,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" s="3">
         <v>3972</v>
       </c>
@@ -1874,7 +1874,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" s="3">
         <v>3973</v>
       </c>
@@ -1892,7 +1892,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" s="3">
         <v>3980</v>
       </c>
@@ -1910,7 +1910,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" s="3">
         <v>3981</v>
       </c>
@@ -1928,7 +1928,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" s="3">
         <v>3982</v>
       </c>
@@ -1946,7 +1946,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" ht="26.5" x14ac:dyDescent="0.35">
       <c r="A56" s="3">
         <v>9990</v>
       </c>

</xml_diff>

<commit_message>
Add error handling and docstring
</commit_message>
<xml_diff>
--- a/DesheTools/configuration/classifyTypeCover_Key.xlsx
+++ b/DesheTools/configuration/classifyTypeCover_Key.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tauex-my.sharepoint.com/personal/kerenha_tauex_tau_ac_il/Documents/Documents/ArcGIS/Deshe/Deshe/DesheTools/configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{D23FDB1F-E947-4AE8-9F3F-3A1A6BF0CD6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55EF0016-9E72-4C43-888B-4AAF1BB2E384}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{D23FDB1F-E947-4AE8-9F3F-3A1A6BF0CD6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8DB7FC9A-7CA3-4DE5-9EF7-505339F02C60}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B3C06EA-3EF4-4486-8996-A04792A06920}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="cover_type_keys" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -895,7 +895,7 @@
   <dimension ref="A1:F56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>